<commit_message>
logic error in sheettype
</commit_message>
<xml_diff>
--- a/Downloads/JioSaavn Litepivot.xlsx
+++ b/Downloads/JioSaavn Litepivot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -34,87 +34,21 @@
     <t>Minor</t>
   </si>
   <si>
+    <t>Critical</t>
+  </si>
+  <si>
     <t>Normal</t>
   </si>
   <si>
     <t>Major</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Terms and Privacy Page not proper</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Reverse Scrolling in Terms and Privacy Page [Device Specific]</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: On terms &amp; privacy page, the JioSaavn logo is overlapping with the information</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: when the internet is off and you try to login with mobile no, the app Crashes</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Though Song removed from library still shows in library</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: The song and jiotune gets played simultaneously</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite : Copyright years are incorrectly written in several sections.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioSaavn Lite: In help and faq section inconsistencies are seen</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: the page gets stuck on the loading page</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Advertisement is not showing in notification bar(Device Specific)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioSaavn Lite: play radio for carnatic is unresponsive</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Music player in notification panel disappears after clicking on pause and play button</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: The pause button in the player in notification bar is cropped.</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Some Podcasts are unavailable and gives error as couldn't find</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: The song played in previous account remains in the player when user logins using another account.</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite : Player disappears when opened from pop-up view</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite : On Sign up page, Terms of Service and Privacy Policy does not directs any where</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: At the bottom, wrong tab heading is highlighted.</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite:When user logs out and tries to play song from notification bar , user sees a white page</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite : When user tries to play a playlist by clicking on 'Play now', it doesn't play</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite : In setting the profile image outer circle is extremely towards right hence some part is cut</t>
-  </si>
-  <si>
     <t>JioSaavn Lite: There is an unprocessed image below the advertisement.</t>
   </si>
   <si>
     <t>JioSaavn Lite: The "privacy policy" link is missing when display language is Malayalam.</t>
   </si>
   <si>
-    <t>JioSaavn Lite: '&amp;' remains same in settings when app language is changed to Tamil</t>
-  </si>
-  <si>
     <t>JioSaavn Lite: App crashes when user clicks on channel radio</t>
   </si>
   <si>
@@ -127,25 +61,13 @@
     <t>JioSaavn Lite: User gets automatically transferred to the "Genres" page when user has opened a channel in split screen mode.</t>
   </si>
   <si>
-    <t xml:space="preserve">JioSaavn Lite: 'Surprise Me' text overlaps content on search page, when display language is Tamil </t>
-  </si>
-  <si>
     <t>JioSaavn Lite: The advertisement that appears after installing the app does not fit in the screen</t>
   </si>
   <si>
-    <t>JioSaavn Lite: Clicking on request jiotune crashes the app.</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Music Language selections must also be in regional language not only English like app language section.</t>
-  </si>
-  <si>
     <t>JioSaavn Lite: Some texts and buttons in a podcast are in English when another display language is selected.</t>
   </si>
   <si>
     <t>JioSaavn Lite: For few songs the description and the song title is in english even though app language is marathi</t>
-  </si>
-  <si>
-    <t>JioSaavn Lite: Radio not available toast pops up when selected from My Library in Artists section</t>
   </si>
   <si>
     <t>JioSaavn Lite: The banner of the song currently playing in the player is changed as JioSaavn logo if opened in pop up view and also when expanded</t>
@@ -629,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,7 +579,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>13769</v>
+        <v>18015</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -671,13 +593,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>13784</v>
+        <v>18016</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -685,13 +607,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>13785</v>
+        <v>18018</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -699,7 +621,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>13786</v>
+        <v>18019</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -713,13 +635,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>13787</v>
+        <v>18020</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -727,7 +649,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>13788</v>
+        <v>18021</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -741,7 +663,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>13789</v>
+        <v>18023</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -755,13 +677,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>13790</v>
+        <v>18026</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
@@ -769,13 +691,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>13791</v>
+        <v>18027</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
@@ -783,13 +705,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>13792</v>
+        <v>18029</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -797,13 +719,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>13793</v>
+        <v>18030</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>19</v>
@@ -811,13 +733,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>13794</v>
+        <v>18031</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>20</v>
@@ -825,13 +747,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>13795</v>
+        <v>18032</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
@@ -839,13 +761,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>13796</v>
+        <v>18033</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -853,13 +775,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>13797</v>
+        <v>18034</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -867,13 +789,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>13799</v>
+        <v>18035</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -881,13 +803,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>13800</v>
+        <v>18036</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>25</v>
@@ -895,13 +817,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>13801</v>
+        <v>18037</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>26</v>
@@ -909,13 +831,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>13802</v>
+        <v>18038</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>27</v>
@@ -923,7 +845,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>13805</v>
+        <v>18039</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
@@ -937,7 +859,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>13806</v>
+        <v>18040</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -951,13 +873,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>18015</v>
+        <v>18041</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>30</v>
@@ -965,7 +887,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>18016</v>
+        <v>18042</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
@@ -979,13 +901,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>18017</v>
+        <v>18043</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>32</v>
@@ -993,13 +915,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>18018</v>
+        <v>18044</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>33</v>
@@ -1007,13 +929,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>18019</v>
+        <v>18045</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>34</v>
@@ -1021,7 +943,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>18020</v>
+        <v>18046</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
@@ -1035,13 +957,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>18021</v>
+        <v>18047</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>36</v>
@@ -1049,13 +971,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>18022</v>
+        <v>18349</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>37</v>
@@ -1063,7 +985,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>18023</v>
+        <v>18350</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
@@ -1077,13 +999,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>18024</v>
+        <v>18351</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>39</v>
@@ -1091,13 +1013,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>18025</v>
+        <v>18352</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>40</v>
@@ -1105,13 +1027,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>18026</v>
+        <v>18353</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>41</v>
@@ -1119,13 +1041,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>18027</v>
+        <v>18354</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>42</v>
@@ -1133,13 +1055,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>18028</v>
+        <v>18355</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>43</v>
@@ -1147,7 +1069,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>18029</v>
+        <v>18356</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>4</v>
@@ -1161,7 +1083,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>18030</v>
+        <v>18357</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>4</v>
@@ -1175,13 +1097,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>18031</v>
+        <v>18358</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>46</v>
@@ -1189,13 +1111,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>18032</v>
+        <v>18359</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>47</v>
@@ -1203,13 +1125,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>18033</v>
+        <v>18360</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>48</v>
@@ -1217,13 +1139,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>18034</v>
+        <v>18363</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>49</v>
@@ -1231,13 +1153,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>18035</v>
+        <v>18369</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>50</v>
@@ -1245,13 +1167,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>18036</v>
+        <v>18373</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>51</v>
@@ -1259,13 +1181,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>18037</v>
+        <v>18374</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>52</v>
@@ -1273,13 +1195,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>18038</v>
+        <v>18377</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>53</v>
@@ -1287,13 +1209,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>18039</v>
+        <v>18380</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>54</v>
@@ -1301,380 +1223,16 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>18040</v>
+        <v>18384</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="2">
-        <v>18041</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2">
-        <v>18042</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2">
-        <v>18043</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2">
-        <v>18044</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2">
-        <v>18045</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2">
-        <v>18046</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2">
-        <v>18047</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="2">
-        <v>18349</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="2">
-        <v>18350</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="2">
-        <v>18351</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="2">
-        <v>18352</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2">
-        <v>18353</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="2">
-        <v>18354</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="2">
-        <v>18355</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="2">
-        <v>18356</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2">
-        <v>18357</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="2">
-        <v>18358</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2">
-        <v>18359</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2">
-        <v>18360</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2">
-        <v>18363</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2">
-        <v>18369</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2">
-        <v>18373</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="2">
-        <v>18374</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="2">
-        <v>18377</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2">
-        <v>18380</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2">
-        <v>18384</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converted rtc date and created date
</commit_message>
<xml_diff>
--- a/Downloads/JioSaavn Litepivot.xlsx
+++ b/Downloads/JioSaavn Litepivot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -26,6 +26,240 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Terms and Privacy Page not proper</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Reverse Scrolling in Terms and Privacy Page [Device Specific]</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: On terms &amp; privacy page, the JioSaavn logo is overlapping with the information</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: when the internet is off and you try to login with mobile no, the app Crashes</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Though Song removed from library still shows in library</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The song and jiotune gets played simultaneously</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : Copyright years are incorrectly written in several sections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JioSaavn Lite: In help and faq section inconsistencies are seen</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: the page gets stuck on the loading page</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Advertisement is not showing in notification bar(Device Specific)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JioSaavn Lite: play radio for carnatic is unresponsive</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Music player in notification panel disappears after clicking on pause and play button</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The pause button in the player in notification bar is cropped.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Some Podcasts are unavailable and gives error as couldn't find</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The song played in previous account remains in the player when user logins using another account.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : Player disappears when opened from pop-up view</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : On Sign up page, Terms of Service and Privacy Policy does not directs any where</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: At the bottom, wrong tab heading is highlighted.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:When user logs out and tries to play song from notification bar , user sees a white page</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : When user tries to play a playlist by clicking on 'Play now', it doesn't play</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : In setting the profile image outer circle is extremely towards right hence some part is cut</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: There is an unprocessed image below the advertisement.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The "privacy policy" link is missing when display language is Malayalam.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: '&amp;' remains same in settings when app language is changed to Tamil</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: App crashes when user clicks on channel radio</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Content in the app overlap with each other when user switches from split screen mode to normal mode.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The username gets cropped in the Mylibrary section.(Enhancement)</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: User gets automatically transferred to the "Genres" page when user has opened a channel in split screen mode.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JioSaavn Lite: 'Surprise Me' text overlaps content on search page, when display language is Tamil </t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The advertisement that appears after installing the app does not fit in the screen</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Clicking on request jiotune crashes the app.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Music Language selections must also be in regional language not only English like app language section.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Some texts and buttons in a podcast are in English when another display language is selected.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: For few songs the description and the song title is in english even though app language is marathi</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Radio not available toast pops up when selected from My Library in Artists section</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The banner of the song currently playing in the player is changed as JioSaavn logo if opened in pop up view and also when expanded</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:The no results found page is in english even though app language is marathi</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: For other display languages few components remain in English.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: For regional language, the "save" for music language and "Yes/No" for logging out is in English</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Even if on boarding language is Hindi, the toast for "Password does not match!" while signing up is in English while creating account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JioSaavn Lite: For Marathi display language, user can see "My Library" translated text but for English display language only "MyLib" </t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: No option to view the password (eye icon) while signing up [Enhancement]</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: If the user kills the app and then clicks on the song in the notification bar the user is been told to login again</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: If clicked on forgot while logging in, the user is taken to different UI and can play any songs even if not logged in</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: For Regional display language, the description for clear player is in English</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: For regional display language,the toasts for clicking thumbs down icon in channels is in English</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Description below the phone number field while signing up when selected on boarding language is Bhojpuri, gets translated after changing the country code</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: App crashes when played the song from notification tile and clicked on phone number after killing the app from background</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: While selecting the on boarding language the 2nd line of the above description is missing for some languages</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: In channels on clicking the channel kids nothing happens</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: After changing the app language to marathi the set as jiotune option for some song is still in english</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Pop up is in english if a user is adding a song in queue and my app language is marathi</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : Mobile navigation overlaps on the list at the bottom of the screen</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: When the user tries to play the 2nd song from notification bar, first song is been played</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Terms &amp; Conditions  and Privacy Policy not present on 'Login with Email' and 'create account' page</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: There is a green patch observed when user scrolls down the shows list in a podcast.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: User can't scroll over the display language page when app is used in split screen mode.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:If the song is been currently played user can observe that there is a play symbol in the notification bar</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Unable to close the popup of JioTune when opened the app in popup view [Device Specific]</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: The Translation of word "Rainy" is incorrect in some display languages.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Jiotunes not available when switched to Wifi even after ZLA login</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:Few components such as "artist radio" are not been converted into marathi if app language is marathi</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : "TrendingJiotunes" should be separated by spaces.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite : White padding at top is observed on page redirected after clicking "More Trending JioTunes"</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Names of songs and playlists changes to English when user clicks on "More Songs" and "More Playlists".</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: User is not able to pause the song from the notification bar once logged out</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:The text overlaps on the login page if user maximise the app from the freeform mode(Device Specific:Oneplus 8T)</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: When outside app and clicked on the song from notification tray shows "loading data..." indefinitely</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Some text in the login page is cropped when display language is Malayalam.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: "Loading" message must be as per the display language.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Some channels names are incorrect in some display languages.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite:  The translation of some texts is incorrect in languages like Hindi, Marathi, Bhojpuri and Haryanvi.</t>
+  </si>
+  <si>
+    <t>JioSaavn Lite: Unable to click on app's back button and meatball menu</t>
   </si>
 </sst>
 </file>
@@ -90,10 +324,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,7 +629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +655,1028 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
+        <v>13769</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>13784</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>13785</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>13786</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>13787</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
+        <v>13788</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
+        <v>13789</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
+        <v>13790</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
+        <v>13791</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>13792</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>13793</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>13794</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>13795</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>13796</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2">
+        <v>13797</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2">
+        <v>13799</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
+        <v>13800</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>13801</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2">
+        <v>13802</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2">
+        <v>13805</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2">
+        <v>13806</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2">
+        <v>18015</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2">
+        <v>18016</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2">
+        <v>18017</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2">
+        <v>18018</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2">
+        <v>18019</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2">
+        <v>18020</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <v>18021</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2">
+        <v>18022</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2">
+        <v>18023</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2">
+        <v>18024</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2">
+        <v>18025</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2">
+        <v>18026</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2">
+        <v>18027</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2">
+        <v>18028</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2">
+        <v>18029</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2">
+        <v>18030</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2">
+        <v>18031</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2">
+        <v>18032</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2">
+        <v>18033</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2">
+        <v>18034</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2">
+        <v>18035</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2">
+        <v>18036</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2">
+        <v>18037</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2">
+        <v>18038</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2">
+        <v>18039</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2">
+        <v>18040</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2">
+        <v>18041</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2">
+        <v>18042</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2">
+        <v>18043</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2">
+        <v>18044</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2">
+        <v>18045</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2">
+        <v>18046</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2">
+        <v>18047</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2">
+        <v>18349</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2">
+        <v>18350</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2">
+        <v>18351</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2">
+        <v>18352</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2">
+        <v>18353</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2">
+        <v>18354</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2">
+        <v>18355</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2">
+        <v>18356</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2">
+        <v>18357</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2">
+        <v>18358</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2">
+        <v>18359</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2">
+        <v>18360</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2">
+        <v>18363</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2">
+        <v>18369</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2">
+        <v>18373</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2">
+        <v>18374</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="2">
+        <v>18377</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="2">
+        <v>18380</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2">
+        <v>18384</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>